<commit_message>
Actually got rid of the switches in RobotSystemsGroup
</commit_message>
<xml_diff>
--- a/UsagebySystem.xlsx
+++ b/UsagebySystem.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="176" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="198" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>AutoRewind</t>
   </si>
@@ -71,13 +71,7 @@
     <t>Shooter Winch Motor</t>
   </si>
   <si>
-    <t>Initial Shooter Limit Switch</t>
-  </si>
-  <si>
-    <t>Final Shooter Limit Switch 1</t>
-  </si>
-  <si>
-    <t>Final Shooter Limit Switch 2</t>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -184,7 +178,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -222,6 +216,10 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -302,10 +300,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:10"/>
+  <dimension ref="1:8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="K9" activeCellId="0" pane="topLeft" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -461,55 +459,34 @@
       <c r="M7" s="2"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="2"/>
+      <c r="A8" s="10"/>
+      <c r="C8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
+comment status manager. Shooter winch won't start unless no final switches pressed
</commit_message>
<xml_diff>
--- a/UsagebySystem.xlsx
+++ b/UsagebySystem.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>AutoRewind</t>
   </si>
@@ -120,14 +120,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FF66"/>
-        <bgColor rgb="FF99CC00"/>
+        <fgColor rgb="FFFF00CC"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00CC"/>
-        <bgColor rgb="FFFF00FF"/>
+        <fgColor rgb="FF99FF66"/>
+        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -207,15 +207,15 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -303,7 +303,7 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100">
-      <selection activeCell="K9" activeCellId="0" pane="topLeft" sqref="K9"/>
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -361,34 +361,34 @@
         <v>12</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="2"/>
+      <c r="M3" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
       <c r="A4" s="5" t="s">
@@ -411,55 +411,58 @@
       <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8">
       <c r="A8" s="10"/>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="0" t="s">
         <v>18</v>
       </c>
@@ -482,6 +485,9 @@
         <v>18</v>
       </c>
       <c r="K8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="0" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="0" t="s">

</xml_diff>

<commit_message>
Eliminated dependence on strings and hardcoded kForward/kReverse
</commit_message>
<xml_diff>
--- a/UsagebySystem.xlsx
+++ b/UsagebySystem.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>AutoRewind</t>
   </si>
@@ -303,7 +303,7 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100">
-      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
+      <selection activeCell="AF18" activeCellId="0" pane="topLeft" sqref="AF18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -460,9 +460,6 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8">
       <c r="A8" s="10"/>
-      <c r="B8" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="C8" s="0" t="s">
         <v>18</v>
       </c>

</xml_diff>